<commit_message>
Salva faixas de horarios dos periodos individualmete para comparar com mais precisao
</commit_message>
<xml_diff>
--- a/dados/horarios_teste.xlsx
+++ b/dados/horarios_teste.xlsx
@@ -55,37 +55,31 @@
       <style:table-row-properties style:row-height="0.841cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro3" style:family="table-row">
-      <style:table-row-properties style:row-height="0.855cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="0.921cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro4" style:family="table-row">
-      <style:table-row-properties style:row-height="0.921cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+      <style:table-row-properties style:row-height="1.058cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro5" style:family="table-row">
-      <style:table-row-properties style:row-height="1.058cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+      <style:table-row-properties style:row-height="0.919cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro6" style:family="table-row">
-      <style:table-row-properties style:row-height="0.919cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+      <style:table-row-properties style:row-height="1.03cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro7" style:family="table-row">
-      <style:table-row-properties style:row-height="1.03cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+      <style:table-row-properties style:row-height="0.863cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro8" style:family="table-row">
-      <style:table-row-properties style:row-height="0.863cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
+      <style:table-row-properties style:row-height="2.868cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
     </style:style>
     <style:style style:name="ro9" style:family="table-row">
-      <style:table-row-properties style:row-height="2.027cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="1.632cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro10" style:family="table-row">
-      <style:table-row-properties style:row-height="1.236cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="2.422cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ro11" style:family="table-row">
-      <style:table-row-properties style:row-height="2.868cm" fo:break-before="auto" style:use-optimal-row-height="false"/>
-    </style:style>
-    <style:style style:name="ro12" style:family="table-row">
-      <style:table-row-properties style:row-height="1.632cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
-    </style:style>
-    <style:style style:name="ro13" style:family="table-row">
-      <style:table-row-properties style:row-height="2.422cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
+      <style:table-row-properties style:row-height="1.236cm" fo:break-before="auto" style:use-optimal-row-height="true"/>
     </style:style>
     <style:style style:name="ta1" style:family="table" style:master-page-name="Default">
       <style:table-properties table:display="true" style:writing-mode="lr-tb"/>
@@ -1547,7 +1541,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0603</text:p>
           </table:table-cell>
@@ -1571,7 +1565,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0679</text:p>
           </table:table-cell>
@@ -1595,7 +1589,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0601</text:p>
           </table:table-cell>
@@ -1619,7 +1613,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1053</text:p>
           </table:table-cell>
@@ -1668,7 +1662,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA0689</text:p>
           </table:table-cell>
@@ -1694,7 +1688,7 @@
           <table:table-cell table:style-name="ce13" table:number-columns-repeated="1008"/>
           <table:table-cell table:number-columns-repeated="8"/>
         </table:table-row>
-        <table:table-row table:style-name="ro3">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1104</text:p>
           </table:table-cell>
@@ -1719,7 +1713,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0606</text:p>
           </table:table-cell>
@@ -1767,7 +1761,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0684</text:p>
           </table:table-cell>
@@ -1791,7 +1785,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0686</text:p>
           </table:table-cell>
@@ -1815,7 +1809,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS0687</text:p>
           </table:table-cell>
@@ -1863,7 +1857,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1047</text:p>
           </table:table-cell>
@@ -1887,7 +1881,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0685</text:p>
           </table:table-cell>
@@ -1911,7 +1905,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0607</text:p>
           </table:table-cell>
@@ -1935,7 +1929,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCB0608</text:p>
           </table:table-cell>
@@ -1959,7 +1953,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0683</text:p>
           </table:table-cell>
@@ -1983,7 +1977,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA0683</text:p>
           </table:table-cell>
@@ -2199,7 +2193,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro4">
+        <table:table-row table:style-name="ro3">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA225</text:p>
           </table:table-cell>
@@ -2223,7 +2217,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro5">
+        <table:table-row table:style-name="ro4">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA041</text:p>
           </table:table-cell>
@@ -2247,7 +2241,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro5">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCS091</text:p>
           </table:table-cell>
@@ -2535,7 +2529,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro7">
+        <table:table-row table:style-name="ro6">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA282</text:p>
           </table:table-cell>
@@ -2563,7 +2557,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro7">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCA283</text:p>
           </table:table-cell>
@@ -2593,7 +2587,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro8">
+        <table:table-row table:style-name="ro7">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX1087</text:p>
           </table:table-cell>
@@ -2621,7 +2615,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro6">
+        <table:table-row table:style-name="ro5">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEX003</text:p>
           </table:table-cell>
@@ -3417,7 +3411,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA019</text:p>
           </table:table-cell>
@@ -3499,7 +3493,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN193</text:p>
           </table:table-cell>
@@ -3765,46 +3759,50 @@
         </table:table-row>
         <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GCH293</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>INTRODUÇÃO À FILOSOFIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="60" calcext:value-type="float">
-            <text:p>60</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>HISTÓRIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
-            <text:p>3</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>3N1234 (04/03/2024 - 06/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
-            <text:p>50</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1017"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro1">
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GCH368</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>TEORIA E METODOLOGIA DA HISTÓRIA I</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="60" calcext:value-type="float">
-            <text:p>60</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>HISTÓRIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="3" calcext:value-type="float">
-            <text:p>3</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>6N1234 (04/03/2024 - 13/07/2024)</text:p>
+            <text:p>GCS238</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>MEIO AMBIENTE, ECONOMIA E SOCIEDADE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="60" calcext:value-type="float">
+            <text:p>60</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>CIÊNCIA DA COMPUTAÇÃO</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="7" calcext:value-type="float">
+            <text:p>7</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>
+              4T12345 (04/03/2024 - 15/06/2024), 
+              <text:s/>
+              4T12 (17/06/2024 - 22/06/2024)
+            </text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1017"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro1">
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>GEX395</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>CÁLCULO NUMÉRICO</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="60" calcext:value-type="float">
+            <text:p>60</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>CIÊNCIA DA COMPUTAÇÃO</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="7" calcext:value-type="float">
+            <text:p>7</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>2T45 4T123 (04/03/2024 - 15/06/2024)</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
             <text:p>50</text:p>
@@ -3867,7 +3865,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GLA553</text:p>
           </table:table-cell>
@@ -4047,7 +4045,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH839</text:p>
           </table:table-cell>
@@ -4071,7 +4069,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA197</text:p>
           </table:table-cell>
@@ -4123,7 +4121,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA285</text:p>
           </table:table-cell>
@@ -4155,7 +4153,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro9">
+        <table:table-row table:style-name="ro2">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA286</text:p>
           </table:table-cell>
@@ -4197,7 +4195,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA291</text:p>
           </table:table-cell>
@@ -4281,7 +4279,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GSA289</text:p>
           </table:table-cell>
@@ -4353,7 +4351,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1120</text:p>
           </table:table-cell>
@@ -4377,7 +4375,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro11">
+        <table:table-row table:style-name="ro8">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH162</text:p>
           </table:table-cell>
@@ -4401,7 +4399,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1123</text:p>
           </table:table-cell>
@@ -4425,7 +4423,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1124</text:p>
           </table:table-cell>
@@ -4449,7 +4447,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1017"/>
         </table:table-row>
-        <table:table-row table:style-name="ro2">
+        <table:table-row table:style-name="ro1">
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GCH1125</text:p>
           </table:table-cell>
@@ -4534,7 +4532,7 @@
           <table:table-cell table:style-name="ce27" table:number-columns-repeated="1008"/>
           <table:table-cell table:style-name="ce28"/>
         </table:table-row>
-        <table:table-row table:style-name="ro12">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4582,7 +4580,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro12">
+        <table:table-row table:style-name="ro9">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4621,100 +4619,6 @@
           </table:table-cell>
           <table:table-cell office:value-type="float" office:value="15" calcext:value-type="float">
             <text:p>15</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ABERTA</text:p>
-          </table:table-cell>
-          <table:covered-table-cell table:style-name="ce19"/>
-          <table:table-cell table:number-columns-repeated="1009"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro13">
-          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
-            <text:p>2024</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
-            <text:p>1501</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>AGRONOMIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GEX1104</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51863" calcext:value-type="float">
-            <text:p>51863</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
-            <text:p>25</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ABERTA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="101" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
-            <text:p>101</text:p>
-          </table:table-cell>
-          <table:table-cell table:number-columns-repeated="1009"/>
-        </table:table-row>
-        <table:table-row table:style-name="ro13">
-          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
-            <text:p>2024</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
-            <text:p>1501</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>AGRONOMIA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>GEX1104</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
-            <text:p>75</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="51865" calcext:value-type="float">
-            <text:p>51865</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
-            <text:p>1</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
-            <text:p>50</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="string" calcext:value-type="string">
-            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
-          </table:table-cell>
-          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
-            <text:p>30</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>ABERTA</text:p>
@@ -4736,6 +4640,100 @@
             <text:p>AGRONOMIA</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>GEX1104</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51863" calcext:value-type="float">
+            <text:p>51863</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>3M45 4M23 (04/03/2024 - 06/07/2024), 3M4 4M2 (08/07/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="25" calcext:value-type="float">
+            <text:p>25</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ABERTA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="101" calcext:value-type="float" table:number-columns-spanned="1" table:number-rows-spanned="2">
+            <text:p>101</text:p>
+          </table:table-cell>
+          <table:table-cell table:number-columns-repeated="1009"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro10">
+          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
+            <text:p>2024</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
+            <text:p>1501</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>AGRONOMIA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>GEX1104</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>QUÍMICA GERAL E INORGÂNICA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="75" calcext:value-type="float">
+            <text:p>75</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="51865" calcext:value-type="float">
+            <text:p>51865</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>34M45 (04/03/2024 - 06/07/2024), 34M4 (08/07/2024 - 13/07/2024)</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="50" calcext:value-type="float">
+            <text:p>50</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ARLINDO CRISTIANO FELIPPE</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="30" calcext:value-type="float">
+            <text:p>30</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>ABERTA</text:p>
+          </table:table-cell>
+          <table:covered-table-cell table:style-name="ce19"/>
+          <table:table-cell table:number-columns-repeated="1009"/>
+        </table:table-row>
+        <table:table-row table:style-name="ro11">
+          <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
+            <text:p>2024</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1" calcext:value-type="float">
+            <text:p>1</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="float" office:value="1501" calcext:value-type="float">
+            <text:p>1501</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
+            <text:p>AGRONOMIA</text:p>
+          </table:table-cell>
+          <table:table-cell office:value-type="string" calcext:value-type="string">
             <text:p>GEN081</text:p>
           </table:table-cell>
           <table:table-cell office:value-type="string" calcext:value-type="string">
@@ -4770,7 +4768,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro10">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4822,7 +4820,7 @@
           <table:covered-table-cell table:style-name="ce19"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro11">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4870,7 +4868,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro11">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4916,7 +4914,7 @@
           <table:covered-table-cell table:style-name="ce19"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro11">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -4964,7 +4962,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro10">
+        <table:table-row table:style-name="ro11">
           <table:table-cell office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -5010,7 +5008,7 @@
           <table:covered-table-cell table:style-name="ce19"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro10">
           <table:table-cell table:style-name="ce12" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -5058,7 +5056,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro10">
           <table:table-cell table:style-name="ce12" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -5104,7 +5102,7 @@
           <table:covered-table-cell table:style-name="ce25"/>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro10">
           <table:table-cell table:style-name="ce12" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -5152,7 +5150,7 @@
           </table:table-cell>
           <table:table-cell table:number-columns-repeated="1009"/>
         </table:table-row>
-        <table:table-row table:style-name="ro13">
+        <table:table-row table:style-name="ro10">
           <table:table-cell table:style-name="ce12" office:value-type="float" office:value="2024" calcext:value-type="float">
             <text:p>2024</text:p>
           </table:table-cell>
@@ -5218,9 +5216,9 @@
 <office:document-meta xmlns:grddl="http://www.w3.org/2003/g/data-view#" xmlns:meta="urn:oasis:names:tc:opendocument:xmlns:meta:1.0" xmlns:xlink="http://www.w3.org/1999/xlink" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:ooo="http://openoffice.org/2004/office" xmlns:office="urn:oasis:names:tc:opendocument:xmlns:office:1.0" office:version="1.2">
   <office:meta>
     <meta:generator>LibreOffice/6.4.7.2$Linux_X86_64 LibreOffice_project/40$Build-2</meta:generator>
-    <dc:date>2024-05-20T15:30:51.874416479</dc:date>
-    <meta:editing-duration>PT3H46M</meta:editing-duration>
-    <meta:editing-cycles>34</meta:editing-cycles>
+    <dc:date>2024-05-21T11:13:29.943705279</dc:date>
+    <meta:editing-duration>PT3H47M19S</meta:editing-duration>
+    <meta:editing-cycles>36</meta:editing-cycles>
     <meta:document-statistic meta:table-count="2" meta:cell-count="1436" meta:object-count="0"/>
   </office:meta>
 </office:document-meta>
@@ -5233,7 +5231,7 @@
       <config:config-item config:name="VisibleAreaTop" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaLeft" config:type="int">0</config:config-item>
       <config:config-item config:name="VisibleAreaWidth" config:type="int">96475</config:config-item>
-      <config:config-item config:name="VisibleAreaHeight" config:type="int">97687</config:config-item>
+      <config:config-item config:name="VisibleAreaHeight" config:type="int">85568</config:config-item>
       <config:config-item-map-indexed config:name="Views">
         <config:config-item-map-entry>
           <config:config-item config:name="ViewId" config:type="string">view1</config:config-item>
@@ -5257,17 +5255,17 @@
               <config:config-item config:name="AnchoredTextOverflowLegacy" config:type="boolean">false</config:config-item>
             </config:config-item-map-entry>
             <config:config-item-map-entry config:name="_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025">
-              <config:config-item config:name="CursorPositionX" config:type="int">4</config:config-item>
-              <config:config-item config:name="CursorPositionY" config:type="int">136</config:config-item>
+              <config:config-item config:name="CursorPositionX" config:type="int">0</config:config-item>
+              <config:config-item config:name="CursorPositionY" config:type="int">147</config:config-item>
               <config:config-item config:name="HorizontalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="VerticalSplitMode" config:type="short">0</config:config-item>
               <config:config-item config:name="HorizontalSplitPosition" config:type="int">0</config:config-item>
               <config:config-item config:name="VerticalSplitPosition" config:type="int">0</config:config-item>
               <config:config-item config:name="ActiveSplitRange" config:type="short">2</config:config-item>
-              <config:config-item config:name="PositionLeft" config:type="int">2</config:config-item>
+              <config:config-item config:name="PositionLeft" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionRight" config:type="int">0</config:config-item>
               <config:config-item config:name="PositionTop" config:type="int">0</config:config-item>
-              <config:config-item config:name="PositionBottom" config:type="int">101</config:config-item>
+              <config:config-item config:name="PositionBottom" config:type="int">113</config:config-item>
               <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
               <config:config-item config:name="ZoomValue" config:type="int">80</config:config-item>
               <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -5276,7 +5274,7 @@
             </config:config-item-map-entry>
           </config:config-item-map-named>
           <config:config-item config:name="ActiveTable" config:type="string">_WITH_docentes_por_turma_AS_SELECT_dt_id_turma_COALESCE_COUNT_p__202402211025</config:config-item>
-          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1861</config:config-item>
+          <config:config-item config:name="HorizontalScrollbarWidth" config:type="int">1836</config:config-item>
           <config:config-item config:name="ZoomType" config:type="short">0</config:config-item>
           <config:config-item config:name="ZoomValue" config:type="int">80</config:config-item>
           <config:config-item config:name="PageViewZoomValue" config:type="int">60</config:config-item>
@@ -5313,7 +5311,7 @@
       <config:config-item config:name="HasColumnRowHeaders" config:type="boolean">true</config:config-item>
       <config:config-item config:name="ShowNotes" config:type="boolean">true</config:config-item>
       <config:config-item config:name="HasSheetTabs" config:type="boolean">true</config:config-item>
-      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpEdXBsZXg6Tm9uZQBQYWdlU2l6ZTpBNAAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
+      <config:config-item config:name="PrinterSetup" config:type="base64Binary">nwH+/0dlbmVyaWMgUHJpbnRlcgAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAU0dFTlBSVAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAAWAAMAwAAAAAAAAAAEAAhSAAAEdAAASm9iRGF0YSAxCnByaW50ZXI9R2VuZXJpYyBQcmludGVyCm9yaWVudGF0aW9uPVBvcnRyYWl0CmNvcGllcz0xCmNvbGxhdGU9ZmFsc2UKbWFyZ2luZGFqdXN0bWVudD0wLDAsMCwwCmNvbG9yZGVwdGg9MjQKcHNsZXZlbD0wCnBkZmRldmljZT0xCmNvbG9yZGV2aWNlPTAKUFBEQ29udGV4RGF0YQpQYWdlU2l6ZTpBNABEdXBsZXg6Tm9uZQAAEgBDT01QQVRfRFVQTEVYX01PREUPAER1cGxleE1vZGU6Ok9mZg==</config:config-item>
       <config:config-item config:name="RasterResolutionX" config:type="int">1000</config:config-item>
       <config:config-item config:name="SyntaxStringRef" config:type="short">7</config:config-item>
       <config:config-item config:name="RasterIsVisible" config:type="boolean">false</config:config-item>
@@ -5475,9 +5473,9 @@
         </style:region-left>
         <style:region-right>
           <text:p>
-            <text:date style:data-style-name="N2" text:date-value="2024-05-20">00/00/0000</text:date>
+            <text:date style:data-style-name="N2" text:date-value="2024-05-21">00/00/0000</text:date>
             , 
-            <text:time style:data-style-name="N2" text:time-value="14:57:36.469775576">00:00:00</text:time>
+            <text:time style:data-style-name="N2" text:time-value="11:12:09.685757207">00:00:00</text:time>
           </text:p>
         </style:region-right>
       </style:header>

</xml_diff>